<commit_message>
working on productline request.
</commit_message>
<xml_diff>
--- a/hierarchy/static/hierarchy/downloads/product-template.xlsx
+++ b/hierarchy/static/hierarchy/downloads/product-template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,15 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20160" yWindow="18740" windowWidth="21780" windowHeight="8620"/>
+    <workbookView xWindow="26300" yWindow="12140" windowWidth="21780" windowHeight="8620"/>
   </bookViews>
   <sheets>
     <sheet name="Product_Hierarchy" sheetId="1" r:id="rId1"/>
     <sheet name="Example" sheetId="6" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Product_Hierarchy!$A$1:$D$1</definedName>
-  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -31,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Igor Item Class</t>
   </si>
@@ -39,115 +36,61 @@
     <t>Usage</t>
   </si>
   <si>
-    <t>EDW</t>
-  </si>
-  <si>
-    <t>FIN</t>
-  </si>
-  <si>
-    <t>FIN ADJ</t>
-  </si>
-  <si>
     <t>E1 Only</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>SAP &amp; E1</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>1LK</t>
   </si>
   <si>
     <t>CELLOMICS SOFTWARE</t>
   </si>
   <si>
-    <t>1LQ</t>
-  </si>
-  <si>
     <t>STORAGE PLATES</t>
   </si>
   <si>
     <t>2SP</t>
   </si>
   <si>
-    <t>92A</t>
-  </si>
-  <si>
-    <t>6SD</t>
-  </si>
-  <si>
-    <t>OEM CE ACCESSORY</t>
-  </si>
-  <si>
-    <t>OEY</t>
-  </si>
-  <si>
-    <t>6SB</t>
-  </si>
-  <si>
-    <t>OEM CE INSTRUMENTS</t>
-  </si>
-  <si>
-    <t>OEI</t>
-  </si>
-  <si>
-    <t>6SC</t>
-  </si>
-  <si>
-    <t>OEM CE SOFTWARE</t>
-  </si>
-  <si>
-    <t>OES</t>
-  </si>
-  <si>
-    <t>HID WF AUTOMATION INSTRUMENTS</t>
-  </si>
-  <si>
-    <t>FHY</t>
-  </si>
-  <si>
-    <t>F4C</t>
-  </si>
-  <si>
-    <t>FHZ</t>
-  </si>
-  <si>
-    <t>HID WF AUTOMATION CONSUMABLES</t>
-  </si>
-  <si>
-    <t>F4B</t>
-  </si>
-  <si>
-    <t>ZJY</t>
-  </si>
-  <si>
-    <t>1LR</t>
-  </si>
-  <si>
-    <t>Igor or Sub PL</t>
-  </si>
-  <si>
     <t>Igor / Sub PL Description</t>
   </si>
   <si>
-    <t>Existing Product Line Code</t>
-  </si>
-  <si>
-    <t>PRODUCT TEMPLATE</t>
+    <t>Product Line Group Code</t>
+  </si>
+  <si>
+    <t>Product Line Name</t>
+  </si>
+  <si>
+    <t>CAS</t>
+  </si>
+  <si>
+    <t>MBL</t>
+  </si>
+  <si>
+    <t>New Name A this is getting to be lorum ipsum</t>
+  </si>
+  <si>
+    <t>New Name B as;ldfjk as;lkdfj ;alsdjk f;lksajd f;lkjasd ;fjk as;lkf kjsad</t>
+  </si>
+  <si>
+    <t>E1&amp;SAP</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>IGOR sublclasdf;ljakdjf;lkjas;dlfkja;slkdjfsd1234</t>
+  </si>
+  <si>
+    <t>Subpldesc890890890890</t>
+  </si>
+  <si>
+    <t>E1blah blah blah blahb lah</t>
   </si>
 </sst>
 </file>
@@ -237,7 +180,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -258,15 +201,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -276,6 +234,13 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -285,6 +250,13 @@
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Product_Hierarchy" xfId="1"/>
   </cellStyles>
@@ -585,50 +557,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="20" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -639,182 +647,117 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on product line
</commit_message>
<xml_diff>
--- a/hierarchy/static/hierarchy/downloads/product-template.xlsx
+++ b/hierarchy/static/hierarchy/downloads/product-template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26300" yWindow="12140" windowWidth="21780" windowHeight="8620"/>
+    <workbookView xWindow="17740" yWindow="18980" windowWidth="21780" windowHeight="8620"/>
   </bookViews>
   <sheets>
     <sheet name="Product_Hierarchy" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Igor / Sub PL Description</t>
   </si>
   <si>
-    <t>Product Line Group Code</t>
-  </si>
-  <si>
     <t>Product Line Name</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>New Name B as;ldfjk as;lkdfj ;alsdjk f;lksajd f;lkjasd ;fjk as;lkf kjsad</t>
   </si>
   <si>
-    <t>E1&amp;SAP</t>
-  </si>
-  <si>
     <t>E1</t>
   </si>
   <si>
@@ -91,6 +85,12 @@
   </si>
   <si>
     <t>E1blah blah blah blahb lah</t>
+  </si>
+  <si>
+    <t>Existing Product Line Group Code</t>
+  </si>
+  <si>
+    <t>SAP &amp; E2</t>
   </si>
 </sst>
 </file>
@@ -180,9 +180,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="34">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -224,7 +226,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="34">
+  <cellStyles count="36">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -241,6 +243,7 @@
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -257,6 +260,7 @@
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Product_Hierarchy" xfId="1"/>
   </cellStyles>
@@ -561,7 +565,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -576,10 +580,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -593,47 +597,47 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -647,7 +651,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -661,10 +665,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -678,7 +682,7 @@
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -692,7 +696,7 @@
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>

</xml_diff>